<commit_message>
content of english files changed (cc/bi and NIF) + the files' names, readmes merged
</commit_message>
<xml_diff>
--- a/en/private/Synthetic/en_p_Synthetic-2.xlsx
+++ b/en/private/Synthetic/en_p_Synthetic-2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedjm\Desktop\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pedjm\Dropbox\Dropbox\GDPR_thesis\Training set\git\Training Set\en\private\Synthetic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAE0B051-0260-4466-AE77-D9810B9AF24C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AFE438EA-94B0-47C5-9DB4-02E5ED01E799}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7350" xr2:uid="{767BAA37-0D6A-40B8-95A9-5E6EBBCB1E31}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>cc</t>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -381,9 +381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F685B9-2E1C-4721-9AAC-8B27FA2EE557}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>